<commit_message>
Adding stock price examples
</commit_message>
<xml_diff>
--- a/datasets/economic/CarsIreland.xlsx
+++ b/datasets/economic/CarsIreland.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jim/Dropbox/R Projects/CT1100/datasets/economic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5D613C-4DB3-8641-A297-767F98FC6202}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6562723A-0A46-F044-9351-8F415105E42D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8080" yWindow="460" windowWidth="28700" windowHeight="16260" xr2:uid="{E6B4AFC9-E651-C04C-B86F-189B9BBEE8E6}"/>
+    <workbookView xWindow="100" yWindow="460" windowWidth="28700" windowHeight="16260" xr2:uid="{E6B4AFC9-E651-C04C-B86F-189B9BBEE8E6}"/>
   </bookViews>
   <sheets>
     <sheet name="New Private Cars" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -514,8 +514,9 @@
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="8" width="10.83203125" style="6"/>
-    <col min="9" max="9" width="14.1640625" style="6" customWidth="1"/>
-    <col min="10" max="11" width="10.83203125" style="6"/>
+    <col min="9" max="9" width="11.5" style="6" customWidth="1"/>
+    <col min="10" max="10" width="10" style="6" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="6"/>
     <col min="12" max="12" width="13.1640625" style="6" customWidth="1"/>
     <col min="13" max="13" width="11.5" style="6" customWidth="1"/>
     <col min="14" max="22" width="10.83203125" style="6"/>

</xml_diff>